<commit_message>
initial time constraints (sem1)
</commit_message>
<xml_diff>
--- a/School of Mathematics - Timetable Data.xlsx
+++ b/School of Mathematics - Timetable Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\topics_in_or\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1402DA-C696-4D30-A4E7-95234795CFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013A6B1D-7DF5-4D3A-A1DD-7833634819C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5472,16 +5472,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.140625" customWidth="1"/>
     <col min="4" max="4" width="82.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>

</xml_diff>